<commit_message>
arrumado a planilha para testar reprovações
</commit_message>
<xml_diff>
--- a/notas_planilha_modelo.xlsx
+++ b/notas_planilha_modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leandroyyy\OneDrive\Fiap\Aula Logica\ponto extra\Entrega-CTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB933B7-C6D3-40EC-809C-843FAF7E6365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2199B31C-937F-4767-85DE-E2AA0E953854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AEC9B240-086D-4A5F-970A-55B671366498}"/>
   </bookViews>
@@ -247,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +348,27 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -869,7 +890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1164,6 +1185,12 @@
     <xf numFmtId="164" fontId="14" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1172,6 +1199,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1489,8 +1519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A175AD0E-438F-491D-98EF-05FF36FEA0E7}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1517,15 +1547,15 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="114"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="116"/>
     </row>
     <row r="3" spans="1:12" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1602,8 +1632,8 @@
       <c r="B5" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="26">
-        <v>7</v>
+      <c r="C5" s="117">
+        <v>2</v>
       </c>
       <c r="D5" s="102">
         <v>8</v>
@@ -1611,11 +1641,11 @@
       <c r="E5" s="103">
         <v>5</v>
       </c>
-      <c r="F5" s="104">
-        <v>9</v>
-      </c>
-      <c r="G5" s="27">
-        <v>9</v>
+      <c r="F5" s="112">
+        <v>0</v>
+      </c>
+      <c r="G5" s="113">
+        <v>4</v>
       </c>
       <c r="H5" s="28">
         <v>6</v>
@@ -3100,6 +3130,7 @@
     <mergeCell ref="D2:J2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>